<commit_message>
poce - TEMPLATE update
</commit_message>
<xml_diff>
--- a/Projects/INBEVNL/Data/POCE_Template.xlsx
+++ b/Projects/INBEVNL/Data/POCE_Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="45">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -67,16 +67,13 @@
     <t xml:space="preserve">Winning Assortment</t>
   </si>
   <si>
-    <t xml:space="preserve">Out of Stock</t>
+    <t xml:space="preserve">Core Assortment</t>
   </si>
   <si>
     <t xml:space="preserve">A,B,C</t>
   </si>
   <si>
     <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Core Assortment</t>
   </si>
   <si>
     <t xml:space="preserve">Planogram HJ Pilsener</t>
@@ -381,20 +378,20 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="A8 A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.7023255813953"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.3209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.24651162790698"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.7209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.43255813953488"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.4558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="41.9162790697674"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="10.9674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,36 +572,36 @@
       </c>
       <c r="G8" s="0"/>
       <c r="H8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
       <c r="H9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>10</v>
@@ -615,21 +612,21 @@
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
@@ -639,21 +636,21 @@
         <v>2</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
@@ -665,67 +662,67 @@
         <v>7</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>